<commit_message>
Chuc nang dat hang hoan tat
</commit_message>
<xml_diff>
--- a/Product_Backlog.xlsx
+++ b/Product_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\chuyennghiep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F954DEA1-622D-4AC7-A843-6B11FFC5DE04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B32076-F700-4B50-A34A-66378BE39724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Ước lượng công việc của Sprint…</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Xây dựng chức năng đánh giá sản phẩm danh cho khách hàng</t>
+  </si>
+  <si>
+    <t>Là một khách hàng, tôi muốn xem lại danh sách các hóa đơn đã đặt</t>
+  </si>
+  <si>
+    <t>Xây dưng trang quản lý hóa đơn của khách hàng</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:H23"/>
+  <dimension ref="A3:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -640,58 +646,67 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="3">
         <v>3</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
         <v>7</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3">
-        <v>2</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3">
         <v>3</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B20" s="3"/>
@@ -705,10 +720,13 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B23" s="3"/>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A19"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>

</xml_diff>